<commit_message>
feat: introduce agentic pipeline for natural language data export, integrating intent classification, template resolution, caching, and new SQL views.
</commit_message>
<xml_diff>
--- a/Eindafrekening/Eindafrekening Inputs/input_master_2025-12-29.xlsx
+++ b/Eindafrekening/Eindafrekening Inputs/input_master_2025-12-29.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ryanrent.sharepoint.com/sites/RyanRent/Gedeelde documenten/General/01_RyanRent&amp;Co/Aljereau/Eindafrekening Generator/Eindafrekening/Eindafrekening Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_AD21B94DCC1D05312014D9037EFCCD609645B8E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4612D158-23E2-E046-9FAE-B6A0CDCD9CCA}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="11_AD21B94DCC1D05312014D9037EFCCD609645B8E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42A8C963-7A8A-5849-9772-6558F9BED743}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="1337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1436" uniqueCount="1337">
   <si>
     <t>COMPLETENESS DASHBOARD</t>
   </si>
@@ -5513,9 +5513,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AQ199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN11" sqref="AN11"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6779,34 +6781,48 @@
       </c>
     </row>
     <row r="15" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C15" t="s">
+        <v>555</v>
+      </c>
       <c r="D15" s="8" t="str">
         <f>IF(A15="","",VLOOKUP(A15,Lists!$A:$B,2,FALSE))</f>
-        <v/>
-      </c>
-      <c r="E15" s="8" t="str">
+        <v>0089</v>
+      </c>
+      <c r="E15" s="8">
         <f>IF(C15="","",VLOOKUP(C15,Lists!$C:$D,2,FALSE))</f>
-        <v/>
+        <v>50448</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
-      <c r="J15" s="9" t="str">
-        <f>IF(A15="","",IFERROR(VLOOKUP(A15,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L15" s="9" t="str">
+      <c r="H15" s="15">
+        <v>45915</v>
+      </c>
+      <c r="I15" s="15">
+        <v>46011</v>
+      </c>
+      <c r="J15" s="9">
+        <v>1650</v>
+      </c>
+      <c r="L15" s="9">
         <f>IF(A15="","",IFERROR(VLOOKUP(A15,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M15" s="10">
         <v>0.21</v>
       </c>
-      <c r="N15" s="11" t="e">
+      <c r="N15" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O15" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>459.8</v>
       </c>
       <c r="R15" s="12" t="str">
         <f>IF(Q15="","",VLOOKUP(Q15,Lists!$E:$F,2,FALSE))</f>
@@ -6849,9 +6865,15 @@
       </c>
     </row>
     <row r="16" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1327</v>
+      </c>
       <c r="D16" s="8" t="str">
         <f>IF(A16="","",VLOOKUP(A16,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E16" s="8" t="str">
         <f>IF(C16="","",VLOOKUP(C16,Lists!$C:$D,2,FALSE))</f>
@@ -6859,20 +6881,20 @@
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
-      <c r="J16" s="9" t="str">
+      <c r="J16" s="9">
         <f>IF(A16="","",IFERROR(VLOOKUP(A16,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L16" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L16" s="9">
         <f>IF(A16="","",IFERROR(VLOOKUP(A16,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M16" s="10">
         <v>0.21</v>
       </c>
-      <c r="N16" s="11" t="e">
+      <c r="N16" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O16" s="11">
         <f t="shared" si="1"/>
@@ -6918,10 +6940,16 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1327</v>
+      </c>
       <c r="D17" s="8" t="str">
         <f>IF(A17="","",VLOOKUP(A17,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E17" s="8" t="str">
         <f>IF(C17="","",VLOOKUP(C17,Lists!$C:$D,2,FALSE))</f>
@@ -6929,20 +6957,20 @@
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="J17" s="9" t="str">
+      <c r="J17" s="9">
         <f>IF(A17="","",IFERROR(VLOOKUP(A17,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L17" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L17" s="9">
         <f>IF(A17="","",IFERROR(VLOOKUP(A17,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M17" s="10">
         <v>0.21</v>
       </c>
-      <c r="N17" s="11" t="e">
+      <c r="N17" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O17" s="11">
         <f t="shared" si="1"/>
@@ -6988,10 +7016,16 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1336</v>
+      </c>
       <c r="D18" s="8" t="str">
         <f>IF(A18="","",VLOOKUP(A18,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E18" s="8" t="str">
         <f>IF(C18="","",VLOOKUP(C18,Lists!$C:$D,2,FALSE))</f>
@@ -6999,20 +7033,20 @@
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="J18" s="9" t="str">
+      <c r="J18" s="9">
         <f>IF(A18="","",IFERROR(VLOOKUP(A18,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L18" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L18" s="9">
         <f>IF(A18="","",IFERROR(VLOOKUP(A18,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M18" s="10">
         <v>0.21</v>
       </c>
-      <c r="N18" s="11" t="e">
+      <c r="N18" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O18" s="11">
         <f t="shared" si="1"/>
@@ -7058,10 +7092,16 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1335</v>
+      </c>
       <c r="D19" s="8" t="str">
         <f>IF(A19="","",VLOOKUP(A19,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E19" s="8" t="str">
         <f>IF(C19="","",VLOOKUP(C19,Lists!$C:$D,2,FALSE))</f>
@@ -7069,20 +7109,20 @@
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="J19" s="9" t="str">
+      <c r="J19" s="9">
         <f>IF(A19="","",IFERROR(VLOOKUP(A19,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L19" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L19" s="9">
         <f>IF(A19="","",IFERROR(VLOOKUP(A19,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M19" s="10">
         <v>0.21</v>
       </c>
-      <c r="N19" s="11" t="e">
+      <c r="N19" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O19" s="11">
         <f t="shared" si="1"/>
@@ -7128,10 +7168,13 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1226</v>
+      </c>
       <c r="D20" s="8" t="str">
         <f>IF(A20="","",VLOOKUP(A20,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E20" s="8" t="str">
         <f>IF(C20="","",VLOOKUP(C20,Lists!$C:$D,2,FALSE))</f>
@@ -7139,20 +7182,20 @@
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="J20" s="9" t="str">
+      <c r="J20" s="9">
         <f>IF(A20="","",IFERROR(VLOOKUP(A20,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L20" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L20" s="9">
         <f>IF(A20="","",IFERROR(VLOOKUP(A20,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M20" s="10">
         <v>0.21</v>
       </c>
-      <c r="N20" s="11" t="e">
+      <c r="N20" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O20" s="11">
         <f t="shared" si="1"/>
@@ -7198,10 +7241,13 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1226</v>
+      </c>
       <c r="D21" s="8" t="str">
         <f>IF(A21="","",VLOOKUP(A21,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E21" s="8" t="str">
         <f>IF(C21="","",VLOOKUP(C21,Lists!$C:$D,2,FALSE))</f>
@@ -7209,20 +7255,20 @@
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="J21" s="9" t="str">
+      <c r="J21" s="9">
         <f>IF(A21="","",IFERROR(VLOOKUP(A21,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L21" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L21" s="9">
         <f>IF(A21="","",IFERROR(VLOOKUP(A21,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M21" s="10">
         <v>0.21</v>
       </c>
-      <c r="N21" s="11" t="e">
+      <c r="N21" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O21" s="11">
         <f t="shared" si="1"/>
@@ -7268,10 +7314,13 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1226</v>
+      </c>
       <c r="D22" s="8" t="str">
         <f>IF(A22="","",VLOOKUP(A22,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E22" s="8" t="str">
         <f>IF(C22="","",VLOOKUP(C22,Lists!$C:$D,2,FALSE))</f>
@@ -7279,20 +7328,20 @@
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
-      <c r="J22" s="9" t="str">
+      <c r="J22" s="9">
         <f>IF(A22="","",IFERROR(VLOOKUP(A22,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L22" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L22" s="9">
         <f>IF(A22="","",IFERROR(VLOOKUP(A22,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M22" s="10">
         <v>0.21</v>
       </c>
-      <c r="N22" s="11" t="e">
+      <c r="N22" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O22" s="11">
         <f t="shared" si="1"/>
@@ -7338,10 +7387,13 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1226</v>
+      </c>
       <c r="D23" s="8" t="str">
         <f>IF(A23="","",VLOOKUP(A23,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E23" s="8" t="str">
         <f>IF(C23="","",VLOOKUP(C23,Lists!$C:$D,2,FALSE))</f>
@@ -7349,20 +7401,20 @@
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
-      <c r="J23" s="9" t="str">
+      <c r="J23" s="9">
         <f>IF(A23="","",IFERROR(VLOOKUP(A23,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L23" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L23" s="9">
         <f>IF(A23="","",IFERROR(VLOOKUP(A23,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M23" s="10">
         <v>0.21</v>
       </c>
-      <c r="N23" s="11" t="e">
+      <c r="N23" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O23" s="11">
         <f t="shared" si="1"/>
@@ -7408,10 +7460,13 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1226</v>
+      </c>
       <c r="D24" s="8" t="str">
         <f>IF(A24="","",VLOOKUP(A24,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E24" s="8" t="str">
         <f>IF(C24="","",VLOOKUP(C24,Lists!$C:$D,2,FALSE))</f>
@@ -7419,20 +7474,20 @@
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
-      <c r="J24" s="9" t="str">
+      <c r="J24" s="9">
         <f>IF(A24="","",IFERROR(VLOOKUP(A24,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L24" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L24" s="9">
         <f>IF(A24="","",IFERROR(VLOOKUP(A24,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M24" s="10">
         <v>0.21</v>
       </c>
-      <c r="N24" s="11" t="e">
+      <c r="N24" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O24" s="11">
         <f t="shared" si="1"/>
@@ -7478,10 +7533,13 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1226</v>
+      </c>
       <c r="D25" s="8" t="str">
         <f>IF(A25="","",VLOOKUP(A25,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E25" s="8" t="str">
         <f>IF(C25="","",VLOOKUP(C25,Lists!$C:$D,2,FALSE))</f>
@@ -7489,20 +7547,20 @@
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
-      <c r="J25" s="9" t="str">
+      <c r="J25" s="9">
         <f>IF(A25="","",IFERROR(VLOOKUP(A25,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L25" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L25" s="9">
         <f>IF(A25="","",IFERROR(VLOOKUP(A25,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M25" s="10">
         <v>0.21</v>
       </c>
-      <c r="N25" s="11" t="e">
+      <c r="N25" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O25" s="11">
         <f t="shared" si="1"/>
@@ -7548,10 +7606,13 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1226</v>
+      </c>
       <c r="D26" s="8" t="str">
         <f>IF(A26="","",VLOOKUP(A26,Lists!$A:$B,2,FALSE))</f>
-        <v/>
+        <v>0089</v>
       </c>
       <c r="E26" s="8" t="str">
         <f>IF(C26="","",VLOOKUP(C26,Lists!$C:$D,2,FALSE))</f>
@@ -7559,20 +7620,20 @@
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
-      <c r="J26" s="9" t="str">
+      <c r="J26" s="9">
         <f>IF(A26="","",IFERROR(VLOOKUP(A26,Lists!$A:$H,8,FALSE),0))</f>
-        <v/>
-      </c>
-      <c r="L26" s="9" t="str">
+        <v>1650</v>
+      </c>
+      <c r="L26" s="9">
         <f>IF(A26="","",IFERROR(VLOOKUP(A26,Lists!$A:$H,7,FALSE),0))</f>
-        <v/>
+        <v>120</v>
       </c>
       <c r="M26" s="10">
         <v>0.21</v>
       </c>
-      <c r="N26" s="11" t="e">
+      <c r="N26" s="11">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>145.19999999999999</v>
       </c>
       <c r="O26" s="11">
         <f t="shared" si="1"/>
@@ -7618,7 +7679,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D27" s="8" t="str">
         <f>IF(A27="","",VLOOKUP(A27,Lists!$A:$B,2,FALSE))</f>
         <v/>
@@ -7688,7 +7749,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D28" s="8" t="str">
         <f>IF(A28="","",VLOOKUP(A28,Lists!$A:$B,2,FALSE))</f>
         <v/>
@@ -7758,7 +7819,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D29" s="8" t="str">
         <f>IF(A29="","",VLOOKUP(A29,Lists!$A:$B,2,FALSE))</f>
         <v/>
@@ -7828,7 +7889,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D30" s="8" t="str">
         <f>IF(A30="","",VLOOKUP(A30,Lists!$A:$B,2,FALSE))</f>
         <v/>
@@ -7898,7 +7959,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D31" s="8" t="str">
         <f>IF(A31="","",VLOOKUP(A31,Lists!$A:$B,2,FALSE))</f>
         <v/>
@@ -7968,7 +8029,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="4:43" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:43" x14ac:dyDescent="0.2">
       <c r="D32" s="8" t="str">
         <f>IF(A32="","",VLOOKUP(A32,Lists!$A:$B,2,FALSE))</f>
         <v/>
@@ -19816,8 +19877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O393"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A329" workbookViewId="0">
+      <selection activeCell="H356" sqref="H356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27729,7 +27790,7 @@
         <v>120</v>
       </c>
       <c r="H355">
-        <v>0</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="356" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>